<commit_message>
Added SETU document types for TICC-319
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.9.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC481FE9-2EE5-48A1-8E47-A41C5278975C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBFEC86-41AE-438D-98A8-6E80A9F3B0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="689">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2104,6 +2104,57 @@
   </si>
   <si>
     <t>Abstract?</t>
+  </si>
+  <si>
+    <t>SETU HR-XML StaffingOrder v1.4</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:hr-xml:2007:staffingorder:1.0</t>
+  </si>
+  <si>
+    <t>TICC-319</t>
+  </si>
+  <si>
+    <t>http://ns.hr-xml.org/2007-04-15::StaffingOrder##hr-xml@nl-1.4::2.5</t>
+  </si>
+  <si>
+    <t>SETU HR-XML StaffingOrder Status v1.4</t>
+  </si>
+  <si>
+    <t>SETU HR-XML HumanResource v1.4</t>
+  </si>
+  <si>
+    <t>http://ns.hr-xml.org/2007-04-15::HumanResource##hr-xml@nl-1.4::2.5</t>
+  </si>
+  <si>
+    <t>SETU HR-XML HumanResource Status v1.4</t>
+  </si>
+  <si>
+    <t>SETU HR-XML Assignment v1.4.1</t>
+  </si>
+  <si>
+    <t>http://ns.hr-xml.org/2007-04-15::Assignment##hr-xml@nl-1.4.1::2.5</t>
+  </si>
+  <si>
+    <t>SETU HR-XML Assignment Status v1.4</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:hr-xml:2007:humanresource:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:hr-xml:2007:assignment:1.0</t>
+  </si>
+  <si>
+    <t>http://ns.hr-xml.org/2007-04-15::StaffingOrder##hr-xml:status@nl-1.4::2.5</t>
+  </si>
+  <si>
+    <t>http://ns.hr-xml.org/2007-04-15::HumanResource##hr-xml:status@nl-1.4::2.5</t>
+  </si>
+  <si>
+    <t>http://ns.hr-xml.org/2007-04-15::Assignment##hr-xml:status@nl-1.4::2.5</t>
   </si>
 </sst>
 </file>
@@ -2763,11 +2814,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:M253"/>
+  <dimension ref="A1:M259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A223" sqref="A223"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A258" sqref="A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11584,6 +11635,198 @@
         <v>532</v>
       </c>
     </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A254" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C254" t="s">
+        <v>676</v>
+      </c>
+      <c r="D254" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="E254" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H254" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="I254" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J254" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L254" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="M254" s="5" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A255" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C255" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="D255" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="E255" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H255" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="I255" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J255" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L255" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="M255" s="5" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A256" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C256" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="D256" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="E256" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H256" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="I256" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J256" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L256" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="M256" s="5" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A257" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C257" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="D257" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="E257" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H257" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="I257" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J257" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L257" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="M257" s="5" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A258" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="D258" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="E258" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H258" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="I258" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J258" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L258" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="M258" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A259" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C259" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="D259" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="E259" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H259" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="I259" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J259" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L259" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="M259" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M253" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Norwegian Digital post IDs; TICC-331
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.9.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8B2E3F-E822-44F8-8807-0FE9B6022A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0060A5E6-34A3-4F8C-8D93-D61304003C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="710">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2161,6 +2161,66 @@
     <t>TICC-215
 TICC-255
 TICC-342</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:digital::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:utskrift::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:flyttet::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:leveringskvittering::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:feil::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:aapningskvittering::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:mottakskvittering::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:varslingfeiletkvittering::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:digdir.no:2020:innbyggerpost:xsd::innbyggerpost##urn:fdc:digdir.no:2020:innbyggerpost:schema:returpostkvittering::1.0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_DIGITAL_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_UTSKRIFT_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_FLYTTET_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_LEVERINGSKVITTERING_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_FEILKVITTERING_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_AAPNINGSKVITTERING_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_MOTTAKSKVITTERING_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_VARSLINGFEILETKVITTERING_1_0</t>
+  </si>
+  <si>
+    <t>INNBYGGERPOST_DPI_RETURPOSTKVITTERING_1_0</t>
+  </si>
+  <si>
+    <t>TICC-331</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::fake</t>
   </si>
 </sst>
 </file>
@@ -2820,11 +2880,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:M259"/>
+  <dimension ref="A1:M268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H184" sqref="H184"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A260" sqref="A260:A268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11833,6 +11893,294 @@
         <v>684</v>
       </c>
     </row>
+    <row r="260" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C260" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="D260" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E260" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H260" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I260" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J260" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L260" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M260" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A261" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C261" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="D261" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E261" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H261" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I261" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J261" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L261" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M261" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A262" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="D262" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E262" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H262" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I262" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J262" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L262" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M262" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A263" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C263" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="D263" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E263" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H263" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I263" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J263" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L263" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M263" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A264" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="D264" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E264" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H264" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I264" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J264" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L264" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M264" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A265" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="D265" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E265" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H265" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I265" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J265" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L265" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M265" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A266" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="D266" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E266" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H266" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I266" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J266" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L266" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M266" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A267" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="B267" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C267" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="D267" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E267" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H267" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I267" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J267" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L267" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M267" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A268" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="D268" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E268" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="H268" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I268" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J268" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L268" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="M268" s="5" t="s">
+        <v>709</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M253" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Inbyggerpost Proc IDs; TICC-331
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.9.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FFA8F1-15C7-44C8-8413-600810A97BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD44034-E97D-4206-B6D5-1A3CAEA4D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="714">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2214,9 +2214,6 @@
     <t>TICC-331</t>
   </si>
   <si>
-    <t>cenbii-procid-ubl::fake</t>
-  </si>
-  <si>
     <t>TICC-222
 TICC-343</t>
   </si>
@@ -2227,6 +2224,20 @@
   <si>
     <t>TICC-270
 TICC-343</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:digital:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:utskrift:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:flyttet:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:digital:ver1.0
+cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:utskrift:ver1.0
+cenbii-procid-ubl::urn:fdc:digdir.no:2020:profile:egovernment:innbyggerpost:flyttet:ver1.0</t>
   </si>
 </sst>
 </file>
@@ -2891,9 +2902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
   <dimension ref="A1:M268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F228" sqref="F228"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M269" sqref="M269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2910,7 +2921,7 @@
     <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="23"/>
     <col min="12" max="12" width="19.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="81.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="84.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
@@ -9462,7 +9473,7 @@
         <v>45565</v>
       </c>
       <c r="H188" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="I188" s="5" t="b">
         <v>0</v>
@@ -9801,7 +9812,7 @@
         <v>45565</v>
       </c>
       <c r="H198" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I198" s="5" t="b">
         <v>0</v>
@@ -10748,7 +10759,7 @@
         <v>45565</v>
       </c>
       <c r="H225" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="I225" s="5" t="b">
         <v>0</v>
@@ -10859,7 +10870,7 @@
         <v>45565</v>
       </c>
       <c r="H228" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="I228" s="5" t="b">
         <v>0</v>
@@ -11955,7 +11966,7 @@
         <v>602</v>
       </c>
       <c r="M260" s="5" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="261" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -11987,7 +11998,7 @@
         <v>602</v>
       </c>
       <c r="M261" s="5" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="262" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -12019,10 +12030,10 @@
         <v>602</v>
       </c>
       <c r="M262" s="5" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="263" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
         <v>700</v>
       </c>
@@ -12051,10 +12062,10 @@
         <v>602</v>
       </c>
       <c r="M263" s="5" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="264" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
         <v>701</v>
       </c>
@@ -12083,7 +12094,7 @@
         <v>602</v>
       </c>
       <c r="M264" s="5" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
     </row>
     <row r="265" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -12115,7 +12126,7 @@
         <v>602</v>
       </c>
       <c r="M265" s="5" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="266" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -12147,7 +12158,7 @@
         <v>602</v>
       </c>
       <c r="M266" s="5" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="267" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -12179,7 +12190,7 @@
         <v>602</v>
       </c>
       <c r="M267" s="5" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="268" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -12211,7 +12222,7 @@
         <v>602</v>
       </c>
       <c r="M268" s="5" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>